<commit_message>
Update mPay In CloseShop
</commit_message>
<xml_diff>
--- a/src/KE-PDC.Web/wwwroot/assets/templates/CloseShopReport.xlsx
+++ b/src/KE-PDC.Web/wwwroot/assets/templates/CloseShopReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\works\ke-pdc\src\KE-PDC.Web\wwwroot\assets\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ke-pdc-web-v2\ke-pdc-web-v2\src\KE-PDC.Web\wwwroot\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69105BE-DE10-46AE-8D70-D012D1181192}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502DA5F0-8ABF-45EB-9C92-F24112139579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-4755" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Close Shop Report" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>AM</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>QR Payment</t>
+  </si>
+  <si>
+    <t>mPay topup</t>
+  </si>
+  <si>
+    <t>rabbit topup</t>
   </si>
 </sst>
 </file>
@@ -182,9 +188,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy\ h:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="[$-1010000]d/m/yyyy\ h:mm:ss;@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -630,10 +636,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -645,10 +651,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -657,7 +663,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="10" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="10" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -681,10 +687,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -693,121 +699,121 @@
     <xf numFmtId="0" fontId="5" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="17" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="19" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="17" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="19" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="20" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="20" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="22" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="22" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="18" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="19" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="19" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="23" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="23" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="13" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="20" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="20" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="22" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="22" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="18" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="19" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="19" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="23" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="23" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="13" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="21" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="18" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="24" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="21" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="18" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="24" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="24" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="24" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="26" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="26" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="26" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="26" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="19" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="19" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="17" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="17" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="25" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="25" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -822,10 +828,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="9" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="9" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="9" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="9" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -858,64 +864,64 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="19" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="19" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="19" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="24" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="9" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="9" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="9" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="13" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="13" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="13" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="10" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="10" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="10" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="25" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="25" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="26" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="26" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="26" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="10" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="19" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="19" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="19" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="24" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="9" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="9" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="9" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="13" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="13" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="13" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="10" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="10" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="10" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="25" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="25" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="26" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="26" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="26" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="10" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="10" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="10" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1300,13 +1306,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX5"/>
+  <dimension ref="A1:AZ5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15"/>
@@ -1323,33 +1329,34 @@
     <col min="15" max="15" width="13.7109375" style="3" customWidth="1"/>
     <col min="16" max="16" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" style="3" customWidth="1"/>
-    <col min="19" max="19" width="21" style="57" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" style="57" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.28515625" style="57" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15" style="29" customWidth="1"/>
-    <col min="23" max="26" width="13.7109375" style="31" customWidth="1"/>
-    <col min="27" max="27" width="16.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.7109375" style="31" customWidth="1"/>
-    <col min="29" max="29" width="15" style="39" customWidth="1"/>
-    <col min="30" max="31" width="19.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="16.28515625" style="4" customWidth="1"/>
-    <col min="34" max="35" width="16.28515625" style="42" customWidth="1"/>
-    <col min="36" max="36" width="13.7109375" style="44" customWidth="1"/>
-    <col min="37" max="40" width="13.7109375" style="21" customWidth="1"/>
-    <col min="41" max="41" width="15" style="37" customWidth="1"/>
-    <col min="42" max="42" width="13.7109375" style="46" customWidth="1"/>
-    <col min="43" max="44" width="13.7109375" style="33" customWidth="1"/>
-    <col min="45" max="45" width="15.85546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15" style="35" customWidth="1"/>
-    <col min="47" max="47" width="18.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.5703125" style="60" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="16" style="62" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8" style="19"/>
-    <col min="51" max="16384" width="8" style="5"/>
+    <col min="18" max="19" width="15" style="3" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" style="3" customWidth="1"/>
+    <col min="21" max="21" width="21" style="57" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.42578125" style="57" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15" style="29" customWidth="1"/>
+    <col min="25" max="28" width="13.7109375" style="31" customWidth="1"/>
+    <col min="29" max="29" width="16.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.7109375" style="31" customWidth="1"/>
+    <col min="31" max="31" width="15" style="39" customWidth="1"/>
+    <col min="32" max="33" width="19.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="16.28515625" style="4" customWidth="1"/>
+    <col min="36" max="37" width="16.28515625" style="42" customWidth="1"/>
+    <col min="38" max="38" width="13.7109375" style="44" customWidth="1"/>
+    <col min="39" max="42" width="13.7109375" style="21" customWidth="1"/>
+    <col min="43" max="43" width="15" style="37" customWidth="1"/>
+    <col min="44" max="44" width="13.7109375" style="46" customWidth="1"/>
+    <col min="45" max="46" width="13.7109375" style="33" customWidth="1"/>
+    <col min="47" max="47" width="15.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="15" style="35" customWidth="1"/>
+    <col min="49" max="49" width="18.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.5703125" style="60" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="16" style="62" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="8" style="19"/>
+    <col min="53" max="16384" width="8" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="14" customFormat="1" ht="25.5" customHeight="1">
+    <row r="1" spans="1:52" s="14" customFormat="1" ht="25.5" customHeight="1">
       <c r="A1" s="65"/>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
@@ -1401,8 +1408,10 @@
       <c r="AU1" s="69"/>
       <c r="AV1" s="69"/>
       <c r="AW1" s="69"/>
+      <c r="AX1" s="69"/>
+      <c r="AY1" s="69"/>
     </row>
-    <row r="2" spans="1:50" s="15" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
+    <row r="2" spans="1:52" s="15" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
       <c r="A2" s="66"/>
       <c r="B2" s="66"/>
       <c r="C2" s="66"/>
@@ -1454,8 +1463,10 @@
       <c r="AU2" s="70"/>
       <c r="AV2" s="70"/>
       <c r="AW2" s="70"/>
+      <c r="AX2" s="70"/>
+      <c r="AY2" s="70"/>
     </row>
-    <row r="3" spans="1:50" s="11" customFormat="1" ht="18.75" customHeight="1">
+    <row r="3" spans="1:52" s="11" customFormat="1" ht="18.75" customHeight="1">
       <c r="A3" s="75" t="s">
         <v>22</v>
       </c>
@@ -1489,51 +1500,53 @@
       <c r="S3" s="84"/>
       <c r="T3" s="84"/>
       <c r="U3" s="84"/>
-      <c r="V3" s="85"/>
-      <c r="W3" s="86" t="s">
+      <c r="V3" s="84"/>
+      <c r="W3" s="84"/>
+      <c r="X3" s="85"/>
+      <c r="Y3" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="X3" s="87"/>
-      <c r="Y3" s="87"/>
       <c r="Z3" s="87"/>
       <c r="AA3" s="87"/>
       <c r="AB3" s="87"/>
-      <c r="AC3" s="88"/>
-      <c r="AD3" s="89" t="s">
+      <c r="AC3" s="87"/>
+      <c r="AD3" s="87"/>
+      <c r="AE3" s="88"/>
+      <c r="AF3" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="AE3" s="90"/>
-      <c r="AF3" s="90"/>
       <c r="AG3" s="90"/>
-      <c r="AH3" s="91"/>
-      <c r="AI3" s="97" t="s">
+      <c r="AH3" s="90"/>
+      <c r="AI3" s="90"/>
+      <c r="AJ3" s="91"/>
+      <c r="AK3" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="AJ3" s="82" t="s">
+      <c r="AL3" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="AK3" s="82"/>
-      <c r="AL3" s="82"/>
       <c r="AM3" s="82"/>
       <c r="AN3" s="82"/>
       <c r="AO3" s="82"/>
-      <c r="AP3" s="94" t="s">
+      <c r="AP3" s="82"/>
+      <c r="AQ3" s="82"/>
+      <c r="AR3" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="AQ3" s="95"/>
-      <c r="AR3" s="95"/>
       <c r="AS3" s="95"/>
-      <c r="AT3" s="96"/>
-      <c r="AU3" s="92" t="s">
+      <c r="AT3" s="95"/>
+      <c r="AU3" s="95"/>
+      <c r="AV3" s="96"/>
+      <c r="AW3" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="AV3" s="93"/>
-      <c r="AW3" s="67" t="s">
+      <c r="AX3" s="93"/>
+      <c r="AY3" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="AX3" s="16"/>
+      <c r="AZ3" s="16"/>
     </row>
-    <row r="4" spans="1:50" s="13" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
+    <row r="4" spans="1:52" s="13" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
       <c r="A4" s="76"/>
       <c r="B4" s="72"/>
       <c r="C4" s="74"/>
@@ -1578,100 +1591,106 @@
         <v>15</v>
       </c>
       <c r="R4" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="S4" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="T4" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="S4" s="54" t="s">
+      <c r="U4" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="T4" s="55" t="s">
+      <c r="V4" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="U4" s="54" t="s">
+      <c r="W4" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="X4" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="W4" s="40" t="s">
+      <c r="Y4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="X4" s="40" t="s">
+      <c r="Z4" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="Y4" s="40" t="s">
+      <c r="AA4" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="Z4" s="40" t="s">
+      <c r="AB4" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="AA4" s="40" t="s">
+      <c r="AC4" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="AB4" s="40" t="s">
+      <c r="AD4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="AC4" s="40" t="s">
+      <c r="AE4" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="AD4" s="12" t="s">
+      <c r="AF4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="AE4" s="12" t="s">
+      <c r="AG4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AF4" s="12" t="s">
+      <c r="AH4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="AG4" s="12" t="s">
+      <c r="AI4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="AH4" s="12" t="s">
+      <c r="AJ4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AI4" s="98"/>
-      <c r="AJ4" s="47" t="s">
+      <c r="AK4" s="98"/>
+      <c r="AL4" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="AK4" s="48" t="s">
+      <c r="AM4" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="AL4" s="48" t="s">
+      <c r="AN4" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="AM4" s="48" t="s">
+      <c r="AO4" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="AN4" s="48" t="s">
+      <c r="AP4" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="AO4" s="48" t="s">
+      <c r="AQ4" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="AP4" s="49" t="s">
+      <c r="AR4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="AQ4" s="50" t="s">
+      <c r="AS4" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="AR4" s="50" t="s">
+      <c r="AT4" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="AS4" s="50" t="s">
+      <c r="AU4" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="AT4" s="50" t="s">
+      <c r="AV4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="AU4" s="58" t="s">
+      <c r="AW4" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="AV4" s="58" t="s">
+      <c r="AX4" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="AW4" s="68"/>
-      <c r="AX4" s="17"/>
+      <c r="AY4" s="68"/>
+      <c r="AZ4" s="17"/>
     </row>
-    <row r="5" spans="1:50" s="10" customFormat="1">
+    <row r="5" spans="1:52" s="10" customFormat="1">
       <c r="A5" s="22"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
@@ -1690,57 +1709,59 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
-      <c r="S5" s="56"/>
-      <c r="T5" s="56"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
       <c r="U5" s="56"/>
-      <c r="V5" s="28"/>
-      <c r="W5" s="30"/>
-      <c r="X5" s="30"/>
+      <c r="V5" s="56"/>
+      <c r="W5" s="56"/>
+      <c r="X5" s="28"/>
       <c r="Y5" s="30"/>
       <c r="Z5" s="30"/>
       <c r="AA5" s="30"/>
       <c r="AB5" s="30"/>
-      <c r="AC5" s="38"/>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="9"/>
+      <c r="AC5" s="30"/>
+      <c r="AD5" s="30"/>
+      <c r="AE5" s="38"/>
       <c r="AF5" s="9"/>
       <c r="AG5" s="9"/>
-      <c r="AH5" s="41"/>
-      <c r="AI5" s="41"/>
-      <c r="AJ5" s="43"/>
-      <c r="AK5" s="20"/>
-      <c r="AL5" s="20"/>
+      <c r="AH5" s="9"/>
+      <c r="AI5" s="9"/>
+      <c r="AJ5" s="41"/>
+      <c r="AK5" s="41"/>
+      <c r="AL5" s="43"/>
       <c r="AM5" s="20"/>
       <c r="AN5" s="20"/>
-      <c r="AO5" s="36"/>
-      <c r="AP5" s="45"/>
-      <c r="AQ5" s="32"/>
-      <c r="AR5" s="32"/>
+      <c r="AO5" s="20"/>
+      <c r="AP5" s="20"/>
+      <c r="AQ5" s="36"/>
+      <c r="AR5" s="45"/>
       <c r="AS5" s="32"/>
-      <c r="AT5" s="34"/>
-      <c r="AU5" s="59"/>
-      <c r="AV5" s="59"/>
-      <c r="AW5" s="61"/>
-      <c r="AX5" s="18"/>
+      <c r="AT5" s="32"/>
+      <c r="AU5" s="32"/>
+      <c r="AV5" s="34"/>
+      <c r="AW5" s="59"/>
+      <c r="AX5" s="59"/>
+      <c r="AY5" s="61"/>
+      <c r="AZ5" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="A1:D2"/>
-    <mergeCell ref="AW3:AW4"/>
-    <mergeCell ref="E1:AW1"/>
-    <mergeCell ref="E2:AW2"/>
+    <mergeCell ref="AY3:AY4"/>
+    <mergeCell ref="E1:AY1"/>
+    <mergeCell ref="E2:AY2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:G3"/>
-    <mergeCell ref="AJ3:AO3"/>
-    <mergeCell ref="H3:V3"/>
-    <mergeCell ref="W3:AC3"/>
-    <mergeCell ref="AD3:AH3"/>
-    <mergeCell ref="AU3:AV3"/>
-    <mergeCell ref="AP3:AT3"/>
-    <mergeCell ref="AI3:AI4"/>
+    <mergeCell ref="AL3:AQ3"/>
+    <mergeCell ref="H3:X3"/>
+    <mergeCell ref="Y3:AE3"/>
+    <mergeCell ref="AF3:AJ3"/>
+    <mergeCell ref="AW3:AX3"/>
+    <mergeCell ref="AR3:AV3"/>
+    <mergeCell ref="AK3:AK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>